<commit_message>
support list with multiple rows in excel
</commit_message>
<xml_diff>
--- a/data/orders_w_id.xlsx
+++ b/data/orders_w_id.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/py/ibportfolio/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D94A7E1-CA2E-A347-BAF6-C527E58159F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B27170C-7041-1540-B251-79DF62467C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15560" xr2:uid="{C8DCFC57-EBDB-ED4A-9025-0DC2B618D6E5}"/>
   </bookViews>
@@ -32,20 +32,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>client_code</t>
   </si>
   <si>
-    <t>funds.fund_id</t>
-  </si>
-  <si>
-    <t>funds.txn_type</t>
-  </si>
-  <si>
-    <t>funds.unit</t>
-  </si>
-  <si>
     <t>settlement_currency</t>
   </si>
   <si>
@@ -76,7 +67,28 @@
     <t>txn_id</t>
   </si>
   <si>
-    <t>obj_id</t>
+    <t>funds-&gt;unit</t>
+  </si>
+  <si>
+    <t>funds-&gt;fund_id</t>
+  </si>
+  <si>
+    <t>bank.branch</t>
+  </si>
+  <si>
+    <t>bank.code</t>
+  </si>
+  <si>
+    <t>9001-5678</t>
+  </si>
+  <si>
+    <t>7002-7890</t>
+  </si>
+  <si>
+    <t>funds-&gt;txn_type</t>
+  </si>
+  <si>
+    <t>msgId</t>
   </si>
 </sst>
 </file>
@@ -451,7 +463,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048A4584-5DC8-5643-9A89-0B128728D18A}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -459,36 +471,44 @@
   <cols>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="18">
+    <row r="2" spans="1:10" ht="18">
       <c r="A2">
         <v>1</v>
       </c>
@@ -496,22 +516,28 @@
         <v>3001</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>123</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2">
         <v>40</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>8</v>
+      <c r="I2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18">
+    <row r="3" spans="1:10" ht="18">
       <c r="A3">
         <v>2</v>
       </c>
@@ -519,22 +545,28 @@
         <v>2001</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>234</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>30</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2">
-        <v>30</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:7" ht="18">
+    <row r="4" spans="1:10" ht="18">
       <c r="A4">
         <v>2</v>
       </c>
@@ -542,22 +574,28 @@
         <v>2001</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>234</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2">
-        <v>50</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="5" spans="1:7" ht="18">
+    <row r="5" spans="1:10" ht="18">
       <c r="A5">
         <v>2</v>
       </c>
@@ -565,19 +603,25 @@
         <v>2001</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>234</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2">
-        <v>10</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix to exclude the col not existing the json template.
</commit_message>
<xml_diff>
--- a/data/orders_w_id.xlsx
+++ b/data/orders_w_id.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/py/ibportfolio/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFF0138-CFB0-184F-BBF7-5F1EF92A61A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42129FC-A6AD-4E4F-9D47-7DE94264C4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15560" xr2:uid="{C8DCFC57-EBDB-ED4A-9025-0DC2B618D6E5}"/>
   </bookViews>
@@ -481,19 +481,23 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18">

</xml_diff>

<commit_message>
bug fix to use copy.deepcopy object instead of copy as it will be pointer for list.
</commit_message>
<xml_diff>
--- a/data/orders_w_id.xlsx
+++ b/data/orders_w_id.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/py/ibportfolio/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42129FC-A6AD-4E4F-9D47-7DE94264C4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A3FC96-37C1-4844-A108-1F1E0E9905E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15560" xr2:uid="{C8DCFC57-EBDB-ED4A-9025-0DC2B618D6E5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>client_code</t>
   </si>
@@ -104,6 +104,18 @@
   </si>
   <si>
     <t>position-&gt;posn_unit</t>
+  </si>
+  <si>
+    <t>C00003</t>
+  </si>
+  <si>
+    <t>6001-7890</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>BA1</t>
   </si>
 </sst>
 </file>
@@ -159,11 +171,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048A4584-5DC8-5643-9A89-0B128728D18A}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -548,7 +561,7 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>123</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -586,7 +599,7 @@
       <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>234</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -624,7 +637,7 @@
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>234</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -663,7 +676,7 @@
       <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>234</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -690,6 +703,45 @@
       <c r="L5">
         <f>H5+50</f>
         <v>60.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4">
+        <v>444</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="2">
+        <v>46.53</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6">
+        <f>H6+50</f>
+        <v>96.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add trailing Zeros to a string
</commit_message>
<xml_diff>
--- a/data/orders_w_id.xlsx
+++ b/data/orders_w_id.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/py/ibportfolio/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A3FC96-37C1-4844-A108-1F1E0E9905E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBA935C-CFBD-784E-82EB-F48044E29DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15560" xr2:uid="{C8DCFC57-EBDB-ED4A-9025-0DC2B618D6E5}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>client_code</t>
   </si>
@@ -116,6 +116,24 @@
   </si>
   <si>
     <t>BA1</t>
+  </si>
+  <si>
+    <t>C00005</t>
+  </si>
+  <si>
+    <t>C00006</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>9001-1234</t>
+  </si>
+  <si>
+    <t>9001-0004</t>
   </si>
 </sst>
 </file>
@@ -491,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048A4584-5DC8-5643-9A89-0B128728D18A}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -586,7 +604,8 @@
         <v>7</v>
       </c>
       <c r="L2">
-        <v>1000</v>
+        <f t="shared" ref="L2:L5" si="0">H2+3000</f>
+        <v>3040</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="18">
@@ -597,22 +616,22 @@
         <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>234</v>
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="2">
-        <v>20.123000000000001</v>
+        <v>10</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>5</v>
@@ -621,36 +640,37 @@
         <v>20</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L3">
-        <v>2020.222</v>
+        <f>H3+4000</f>
+        <v>4010</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>234</v>
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="2">
-        <v>50.226700000000001</v>
+        <v>20</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>5</v>
@@ -659,16 +679,16 @@
         <v>20</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L4">
-        <f>H4+3000</f>
-        <v>3050.2267000000002</v>
+        <f t="shared" si="0"/>
+        <v>3020</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="18">
       <c r="A5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>21</v>
@@ -683,13 +703,13 @@
         <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="2">
-        <v>10.1</v>
+        <v>20.123000000000001</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>5</v>
@@ -698,49 +718,127 @@
         <v>20</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="L5">
-        <f>H5+50</f>
-        <v>60.1</v>
+        <f t="shared" si="0"/>
+        <v>3020.123</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="18">
       <c r="A6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="D6" s="4">
-        <v>444</v>
+        <v>234</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="2">
-        <v>46.53</v>
+        <v>50.226700000000001</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="K6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6">
+        <f>H6+3000</f>
+        <v>3050.2267000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>234</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <f>H7+50</f>
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="18">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4">
+        <v>444</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="2">
+        <v>46.53</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L6">
-        <f>H6+50</f>
+      <c r="L8">
+        <f>H8+50</f>
         <v>96.53</v>
       </c>
     </row>

</xml_diff>